<commit_message>
finish hardware second stage
</commit_message>
<xml_diff>
--- a/Hardware/制作/BOM.xlsx
+++ b/Hardware/制作/BOM.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Catch5Yeah\Hardware\制作\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA792DE6-7C43-4CCA-B7C9-27BA6D1D2D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AFDCEC-CE07-4764-BAC8-7168A16DBC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="紧固件" sheetId="1" r:id="rId1"/>
     <sheet name="铁盒" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">紧固件!$A$1:$E$58</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">紧固件!$A$1:$E$67</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="96">
   <si>
     <t>类别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -360,6 +361,66 @@
   </si>
   <si>
     <t>M4*7*1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侧壁-AC电源插座</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>底板-PCB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M6*16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>顶盖-提手</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M6*20*1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M3*6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>皮带扣</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>螺母位过大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线轮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>凹槽过浅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>吊轮架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>降低皮带扣位置，以防止皮带空转</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>边缘突出底盘侧壁，中部低于侧壁开槽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -367,7 +428,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,14 +445,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C5700"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -400,7 +469,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -413,19 +487,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="差" xfId="2" builtinId="27"/>
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="适中" xfId="1" builtinId="28"/>
+    <cellStyle name="好" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -703,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1180,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
         <v>28</v>
@@ -1139,10 +1218,10 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="1" t="s">
+      <c r="A31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C31" t="s">
@@ -1489,10 +1568,10 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="1" t="s">
+      <c r="A56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C56" t="s">
@@ -1530,8 +1609,134 @@
         <v>4</v>
       </c>
     </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C61" t="s">
+        <v>82</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" t="s">
+        <v>82</v>
+      </c>
+      <c r="D62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" t="s">
+        <v>82</v>
+      </c>
+      <c r="D64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" t="s">
+        <v>84</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C66" t="s">
+        <v>84</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C67" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E58" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1543,7 +1748,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1646,4 +1851,56 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB3B75C-B4D9-4069-94FD-D93BCF69A952}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="78.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finish hardware third stage
</commit_message>
<xml_diff>
--- a/Hardware/制作/BOM.xlsx
+++ b/Hardware/制作/BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Catch5Yeah\Hardware\制作\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63AFDCEC-CE07-4764-BAC8-7168A16DBC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F406FADA-CF01-4372-8713-CA26A728E382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="紧固件" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="104">
   <si>
     <t>类别</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -421,6 +421,38 @@
   </si>
   <si>
     <t>边缘突出底盘侧壁，中部低于侧壁开槽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RGB灯条卡槽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>螺母位过大</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L锁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>突出部分位置过高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>顶盖密码锁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>侧壁密码锁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>密码锁开孔过小；去除弹簧触点支架</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去除弹簧触点支架</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -782,19 +814,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B60" sqref="B59:B60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.35546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -811,7 +844,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -825,7 +858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -839,7 +872,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -853,7 +886,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -867,7 +900,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -881,7 +914,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -895,7 +928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -909,7 +942,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -923,7 +956,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -937,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -951,7 +984,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -965,7 +998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
@@ -979,7 +1012,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>3</v>
       </c>
@@ -993,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>9</v>
       </c>
@@ -1007,7 +1040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -1021,7 +1054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1035,7 +1068,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>11</v>
       </c>
@@ -1049,7 +1082,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>9</v>
       </c>
@@ -1063,7 +1096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1077,7 +1110,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>9</v>
       </c>
@@ -1091,7 +1124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -1105,7 +1138,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1119,7 +1152,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>11</v>
       </c>
@@ -1133,7 +1166,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>11</v>
       </c>
@@ -1161,7 +1194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>9</v>
       </c>
@@ -1175,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>9</v>
       </c>
@@ -1189,7 +1222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>11</v>
       </c>
@@ -1203,7 +1236,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
@@ -1217,7 +1250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>9</v>
       </c>
@@ -1231,7 +1264,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>11</v>
       </c>
@@ -1259,7 +1292,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>11</v>
       </c>
@@ -1273,7 +1306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>9</v>
       </c>
@@ -1287,7 +1320,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>11</v>
       </c>
@@ -1301,7 +1334,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>9</v>
       </c>
@@ -1315,7 +1348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>9</v>
       </c>
@@ -1329,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>11</v>
       </c>
@@ -1343,7 +1376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>9</v>
       </c>
@@ -1357,7 +1390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>9</v>
       </c>
@@ -1371,7 +1404,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>9</v>
       </c>
@@ -1385,7 +1418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>3</v>
       </c>
@@ -1399,7 +1432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>11</v>
       </c>
@@ -1413,7 +1446,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>9</v>
       </c>
@@ -1427,7 +1460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>66</v>
       </c>
@@ -1441,7 +1474,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>66</v>
       </c>
@@ -1455,7 +1488,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>66</v>
       </c>
@@ -1469,7 +1502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>77</v>
       </c>
@@ -1483,7 +1516,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>9</v>
       </c>
@@ -1497,7 +1530,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>11</v>
       </c>
@@ -1511,7 +1544,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>9</v>
       </c>
@@ -1525,7 +1558,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>11</v>
       </c>
@@ -1539,7 +1572,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>11</v>
       </c>
@@ -1553,7 +1586,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>9</v>
       </c>
@@ -1567,7 +1600,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>9</v>
       </c>
@@ -1581,7 +1614,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>11</v>
       </c>
@@ -1595,7 +1628,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>6</v>
       </c>
@@ -1609,7 +1642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>9</v>
       </c>
@@ -1623,7 +1656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>11</v>
       </c>
@@ -1637,7 +1670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>11</v>
       </c>
@@ -1651,7 +1684,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>9</v>
       </c>
@@ -1665,7 +1698,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>6</v>
       </c>
@@ -1679,7 +1712,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>3</v>
       </c>
@@ -1693,7 +1726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>9</v>
       </c>
@@ -1707,7 +1740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>3</v>
       </c>
@@ -1721,7 +1754,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
@@ -1736,7 +1769,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E67" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:E67" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="侧壁-AC电源插座"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1751,12 +1790,12 @@
       <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.109375" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>34</v>
       </c>
@@ -1773,7 +1812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1790,7 +1829,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -1807,7 +1846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1821,7 +1860,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1832,7 +1871,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1855,47 +1894,80 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BB3B75C-B4D9-4069-94FD-D93BCF69A952}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="78.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="78.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>88</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>90</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>92</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>